<commit_message>
Adding raw incidence data to output
</commit_message>
<xml_diff>
--- a/Data/Cancer Trends/Source Data/Raw Data/Cancer_NIreland.xlsx
+++ b/Data/Cancer Trends/Source Data/Raw Data/Cancer_NIreland.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{0D4063F2-4E1B-4688-BF2E-BB48B8503F64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="6" xr2:uid="{74AF0F0E-6CBD-4D76-8062-8F07B8053D2C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="5" xr2:uid="{74AF0F0E-6CBD-4D76-8062-8F07B8053D2C}"/>
   </bookViews>
   <sheets>
     <sheet name="All Cancers Excl. NMSC" sheetId="1" r:id="rId1"/>
@@ -7684,8 +7684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5B347DC-EC8A-4494-824C-907CB3CB0B7D}">
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T17" sqref="T17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8958,8 +8958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A808A83C-66F2-41C2-B87C-B89E0D5EE76E}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>